<commit_message>
Further amendmets to the data set
</commit_message>
<xml_diff>
--- a/dream/KnowledgeExtraction/KEtool_examples/KE tool&GUI/test_data.xlsx
+++ b/dream/KnowledgeExtraction/KEtool_examples/KE tool&GUI/test_data.xlsx
@@ -442,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:P198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="S186" sqref="S186"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +529,7 @@
         <v>0.21430665422460365</v>
       </c>
       <c r="J2" s="6">
-        <v>0.3955889589552477</v>
+        <v>0.40936212999999999</v>
       </c>
       <c r="K2" s="4">
         <v>0.19843493323223443</v>
@@ -573,7 +573,7 @@
         <v>0.18271264720431088</v>
       </c>
       <c r="J3" s="6">
-        <v>0.42649778359616775</v>
+        <v>0.42562534000000002</v>
       </c>
       <c r="K3" s="4">
         <v>0.21274455776912232</v>
@@ -617,7 +617,7 @@
         <v>0.20320609659322039</v>
       </c>
       <c r="J4" s="6">
-        <v>0.39301367057050623</v>
+        <v>0.39069166999999999</v>
       </c>
       <c r="K4" s="4">
         <v>0.18633704936902057</v>
@@ -661,7 +661,7 @@
         <v>0.18694682101538951</v>
       </c>
       <c r="J5" s="6">
-        <v>0.4019453292011545</v>
+        <v>0.38563217999999999</v>
       </c>
       <c r="K5" s="4">
         <v>0.22397557022050191</v>
@@ -705,7 +705,7 @@
         <v>0.20109890704224292</v>
       </c>
       <c r="J6" s="6">
-        <v>0.3845894908703813</v>
+        <v>0.40100604000000001</v>
       </c>
       <c r="K6" s="4">
         <v>0.19445262678826372</v>
@@ -749,7 +749,7 @@
         <v>0.20513816776641247</v>
       </c>
       <c r="J7" s="6">
-        <v>0.39990148762387445</v>
+        <v>0.35835318999999999</v>
       </c>
       <c r="K7" s="4">
         <v>0.21545850419338844</v>
@@ -793,7 +793,7 @@
         <v>0.19742886444462499</v>
       </c>
       <c r="J8" s="6">
-        <v>0.42991191960808406</v>
+        <v>0.39890998</v>
       </c>
       <c r="K8" s="4">
         <v>0.18733962061028808</v>
@@ -837,7 +837,7 @@
         <v>0.18917336257675144</v>
       </c>
       <c r="J9" s="6">
-        <v>0.35665522871161215</v>
+        <v>0.41519472000000002</v>
       </c>
       <c r="K9" s="4">
         <v>0.24954856371376186</v>
@@ -881,7 +881,7 @@
         <v>0.21835937226294436</v>
       </c>
       <c r="J10" s="6">
-        <v>0.41731426652706211</v>
+        <v>0.43680103999999997</v>
       </c>
       <c r="K10" s="4">
         <v>0.17037972567371762</v>
@@ -925,7 +925,7 @@
         <v>0.18925372605729637</v>
       </c>
       <c r="J11" s="6">
-        <v>0.38481283349002104</v>
+        <v>0.39468340000000002</v>
       </c>
       <c r="K11" s="4">
         <v>0.20508218404527631</v>
@@ -969,7 +969,7 @@
         <v>0.19808408965287416</v>
       </c>
       <c r="J12" s="6">
-        <v>0.37993231610889339</v>
+        <v>0.40561253000000003</v>
       </c>
       <c r="K12" s="4">
         <v>0.17232445104995658</v>
@@ -1013,7 +1013,7 @@
         <v>0.20589921402202824</v>
       </c>
       <c r="J13" s="6">
-        <v>0.41232733681357209</v>
+        <v>0.38531048000000001</v>
       </c>
       <c r="K13" s="4">
         <v>0.27148449346309211</v>
@@ -1057,7 +1057,7 @@
         <v>0.20023569816610393</v>
       </c>
       <c r="J14" s="6">
-        <v>0.39231779363347585</v>
+        <v>0.37984444000000001</v>
       </c>
       <c r="K14" s="4">
         <v>0.17596249523602767</v>
@@ -1101,7 +1101,7 @@
         <v>0.19390239986196992</v>
       </c>
       <c r="J15" s="6">
-        <v>0.40258676374187924</v>
+        <v>0.38283815999999998</v>
       </c>
       <c r="K15" s="4">
         <v>0.26139444337955198</v>
@@ -1145,7 +1145,7 @@
         <v>0.20293219720027983</v>
       </c>
       <c r="J16" s="6">
-        <v>0.40945002602018321</v>
+        <v>0.37544364000000002</v>
       </c>
       <c r="K16" s="4">
         <v>0.20980759877318347</v>
@@ -1189,7 +1189,7 @@
         <v>0.21313443690746167</v>
       </c>
       <c r="J17" s="6">
-        <v>0.40997095263105615</v>
+        <v>0.39981849000000003</v>
       </c>
       <c r="K17" s="4">
         <v>0.2652251142613577</v>
@@ -1233,7 +1233,7 @@
         <v>0.19630564676661744</v>
       </c>
       <c r="J18" s="6">
-        <v>0.41297899060037191</v>
+        <v>0.40134747999999998</v>
       </c>
       <c r="K18" s="4">
         <v>0.19298572772375194</v>
@@ -1277,7 +1277,7 @@
         <v>0.22594447288021149</v>
       </c>
       <c r="J19" s="6">
-        <v>0.38863889031096865</v>
+        <v>0.37618108</v>
       </c>
       <c r="K19" s="4">
         <v>0.21279892076733017</v>
@@ -1321,7 +1321,7 @@
         <v>0.18779158924605685</v>
       </c>
       <c r="J20" s="6">
-        <v>0.36120723433801072</v>
+        <v>0.38233539</v>
       </c>
       <c r="K20" s="4">
         <v>0.27332621534699036</v>
@@ -1365,7 +1365,7 @@
         <v>0.19585887698390295</v>
       </c>
       <c r="J21" s="6">
-        <v>0.40259440418188475</v>
+        <v>0.39975722000000002</v>
       </c>
       <c r="K21" s="4">
         <v>0.23105245911138048</v>
@@ -1409,7 +1409,7 @@
         <v>0.18667439091288179</v>
       </c>
       <c r="J22" s="6">
-        <v>0.38825900384656992</v>
+        <v>0.39098460000000002</v>
       </c>
       <c r="K22" s="4">
         <v>0.26596187027150681</v>
@@ -1453,7 +1453,7 @@
         <v>0.21004213453979467</v>
       </c>
       <c r="J23" s="6">
-        <v>0.39907148876884518</v>
+        <v>0.41997444</v>
       </c>
       <c r="K23" s="4">
         <v>0.29780992229057524</v>
@@ -1497,7 +1497,7 @@
         <v>0.19274924206006352</v>
       </c>
       <c r="J24" s="6">
-        <v>0.44750337808537211</v>
+        <v>0.38245828999999998</v>
       </c>
       <c r="K24" s="4">
         <v>0.19147030334893722</v>
@@ -1541,7 +1541,7 @@
         <v>0.20951120705585041</v>
       </c>
       <c r="J25" s="6">
-        <v>0.39839244858792278</v>
+        <v>0.38979007999999998</v>
       </c>
       <c r="K25" s="4">
         <v>0.19349497819337286</v>
@@ -1585,7 +1585,7 @@
         <v>0.19345006811036872</v>
       </c>
       <c r="J26" s="6">
-        <v>0.39405528774714449</v>
+        <v>0.42461687999999997</v>
       </c>
       <c r="K26" s="4">
         <v>0.23236113393098701</v>
@@ -1629,7 +1629,7 @@
         <v>0.20110054935616831</v>
       </c>
       <c r="J27" s="6">
-        <v>0.41037190128367285</v>
+        <v>0.42671687000000003</v>
       </c>
       <c r="K27" s="4">
         <v>0.20765496080417778</v>
@@ -1673,7 +1673,7 @@
         <v>0.20339213410717794</v>
       </c>
       <c r="J28" s="6">
-        <v>0.41856641442475984</v>
+        <v>0.35183238</v>
       </c>
       <c r="K28" s="4">
         <v>0.24427787979084226</v>
@@ -1717,7 +1717,7 @@
         <v>0.19813260402012281</v>
       </c>
       <c r="J29" s="6">
-        <v>0.39855642159334342</v>
+        <v>0.38566781999999999</v>
       </c>
       <c r="K29" s="4">
         <v>0.22389423998855787</v>
@@ -1761,7 +1761,7 @@
         <v>0.19773542071284816</v>
       </c>
       <c r="J30" s="6">
-        <v>0.40430556109404336</v>
+        <v>0.40115520999999998</v>
       </c>
       <c r="K30" s="4">
         <v>0.23866977089282704</v>
@@ -1805,7 +1805,7 @@
         <v>0.20026673130111591</v>
       </c>
       <c r="J31" s="6">
-        <v>0.43001874079423485</v>
+        <v>0.36245261000000001</v>
       </c>
       <c r="K31" s="4">
         <v>0.17544227433030091</v>
@@ -1849,7 +1849,7 @@
         <v>0.19049812699465882</v>
       </c>
       <c r="J32" s="6">
-        <v>0.39158771707663909</v>
+        <v>0.38709126999999999</v>
       </c>
       <c r="K32" s="4">
         <v>0.20428089592736814</v>
@@ -1893,7 +1893,7 @@
         <v>0.21105107264173562</v>
       </c>
       <c r="J33" s="6">
-        <v>0.42450618600089907</v>
+        <v>0.39531882000000002</v>
       </c>
       <c r="K33" s="4">
         <v>0.2586801701810435</v>
@@ -1937,7 +1937,7 @@
         <v>0.19171175353863726</v>
       </c>
       <c r="J34" s="6">
-        <v>0.37255949235024399</v>
+        <v>0.38633925000000002</v>
       </c>
       <c r="K34" s="4">
         <v>0.21305546454594743</v>
@@ -1981,7 +1981,7 @@
         <v>0.19260031855116516</v>
       </c>
       <c r="J35" s="6">
-        <v>0.38772911810864319</v>
+        <v>0.39854440000000002</v>
       </c>
       <c r="K35" s="4">
         <v>0.24654280754983138</v>
@@ -2025,7 +2025,7 @@
         <v>0.198185574427588</v>
       </c>
       <c r="J36" s="6">
-        <v>0.41200422616596466</v>
+        <v>0.41041386000000002</v>
       </c>
       <c r="K36" s="4">
         <v>0.25152047431168723</v>
@@ -2069,7 +2069,7 @@
         <v>0.20171049306188304</v>
       </c>
       <c r="J37" s="6">
-        <v>0.38520388840782049</v>
+        <v>0.36929815999999999</v>
       </c>
       <c r="K37" s="4">
         <v>0.19826461060486567</v>
@@ -2113,7 +2113,7 @@
         <v>0.1944561871035361</v>
       </c>
       <c r="J38" s="6">
-        <v>0.40515210533317003</v>
+        <v>0.40932816</v>
       </c>
       <c r="K38" s="4">
         <v>0.22212339319900742</v>
@@ -2157,7 +2157,7 @@
         <v>0.20238054989814341</v>
       </c>
       <c r="J39" s="6">
-        <v>0.39833570566278925</v>
+        <v>0.40402185000000002</v>
       </c>
       <c r="K39" s="4">
         <v>0.17745812434808028</v>
@@ -2201,7 +2201,7 @@
         <v>0.18802104896579588</v>
       </c>
       <c r="J40" s="6">
-        <v>0.38911702720802194</v>
+        <v>0.40227199000000002</v>
       </c>
       <c r="K40" s="4">
         <v>0.22656611971010715</v>
@@ -2245,7 +2245,7 @@
         <v>0.20560485764523517</v>
       </c>
       <c r="J41" s="6">
-        <v>0.37411053142718609</v>
+        <v>0.38157706000000002</v>
       </c>
       <c r="K41" s="4">
         <v>0.15711785259528421</v>
@@ -2289,7 +2289,7 @@
         <v>0.20304228098311941</v>
       </c>
       <c r="J42" s="6">
-        <v>0.39439177450309421</v>
+        <v>0.36680391000000001</v>
       </c>
       <c r="K42" s="4">
         <v>0.16535621998457464</v>
@@ -2333,7 +2333,7 @@
         <v>0.19755046685454594</v>
       </c>
       <c r="J43" s="6">
-        <v>0.41149910892520541</v>
+        <v>0.37695005999999998</v>
       </c>
       <c r="K43" s="4">
         <v>0.13990379728525601</v>
@@ -2377,7 +2377,7 @@
         <v>0.2005384144257833</v>
       </c>
       <c r="J44" s="6">
-        <v>0.40364879534991288</v>
+        <v>0.40554154999999997</v>
       </c>
       <c r="K44" s="4">
         <v>0.21521424575705939</v>
@@ -2421,7 +2421,7 @@
         <v>0.20970890623364569</v>
       </c>
       <c r="J45" s="6">
-        <v>0.42594369411207972</v>
+        <v>0.45891905999999999</v>
       </c>
       <c r="K45" s="4">
         <v>0.22033290011960341</v>
@@ -2465,7 +2465,7 @@
         <v>0.20724014858317064</v>
       </c>
       <c r="J46" s="6">
-        <v>0.39971295628633108</v>
+        <v>0.35786990000000002</v>
       </c>
       <c r="K46" s="4">
         <v>0.2076058008714628</v>
@@ -2509,7 +2509,7 @@
         <v>0.21053443009139336</v>
       </c>
       <c r="J47" s="6">
-        <v>0.40027577569122647</v>
+        <v>0.39313700000000001</v>
       </c>
       <c r="K47" s="4">
         <v>0.24984229405305719</v>
@@ -2553,7 +2553,7 @@
         <v>0.19467801336768034</v>
       </c>
       <c r="J48" s="6">
-        <v>0.35988960057549924</v>
+        <v>0.41907327</v>
       </c>
       <c r="K48" s="4">
         <v>0.21532947069656266</v>
@@ -2597,7 +2597,7 @@
         <v>0.20561821977432995</v>
       </c>
       <c r="J49" s="6">
-        <v>0.409777304380951</v>
+        <v>0.40600532</v>
       </c>
       <c r="K49" s="4">
         <v>0.21523567319771164</v>
@@ -2641,7 +2641,7 @@
         <v>0.19384029628542973</v>
       </c>
       <c r="J50" s="6">
-        <v>0.42389329869635933</v>
+        <v>0.41578749999999998</v>
       </c>
       <c r="K50" s="4">
         <v>0.27948687151909435</v>
@@ -2685,7 +2685,7 @@
         <v>0.21043439365090186</v>
       </c>
       <c r="J51" s="6">
-        <v>0.39144912176253394</v>
+        <v>0.41802017000000002</v>
       </c>
       <c r="K51" s="4">
         <v>0.18608517647027972</v>
@@ -2729,7 +2729,7 @@
         <v>0.19064735945908595</v>
       </c>
       <c r="J52" s="6">
-        <v>0.39897298438447965</v>
+        <v>0.42433597000000001</v>
       </c>
       <c r="K52" s="4">
         <v>0.22289884918862563</v>
@@ -2773,7 +2773,7 @@
         <v>0.20463215440848523</v>
       </c>
       <c r="J53" s="6">
-        <v>0.40945553144688229</v>
+        <v>0.37530929000000002</v>
       </c>
       <c r="K53" s="4">
         <v>0.24693230293248844</v>
@@ -2817,7 +2817,7 @@
         <v>0.18597092905997487</v>
       </c>
       <c r="J54" s="6">
-        <v>0.41147283109954563</v>
+        <v>0.39991863</v>
       </c>
       <c r="K54" s="4">
         <v>0.24643463646018254</v>
@@ -2861,7 +2861,7 @@
         <v>0.20609544312451711</v>
       </c>
       <c r="J55" s="6">
-        <v>0.39133351287282719</v>
+        <v>0.37627739999999998</v>
       </c>
       <c r="K55" s="4">
         <v>0.25260400894178592</v>
@@ -2905,7 +2905,7 @@
         <v>0.1945497967387895</v>
       </c>
       <c r="J56" s="6">
-        <v>0.40404339145684337</v>
+        <v>0.39246365</v>
       </c>
       <c r="K56" s="4">
         <v>0.10815116173258157</v>
@@ -2949,7 +2949,7 @@
         <v>0.20180616310979041</v>
       </c>
       <c r="J57" s="6">
-        <v>0.37917646756792506</v>
+        <v>0.37695187000000002</v>
       </c>
       <c r="K57" s="4">
         <v>0.20040692961221071</v>
@@ -2993,7 +2993,7 @@
         <v>0.20561489150320084</v>
       </c>
       <c r="J58" s="6">
-        <v>0.3821365113633875</v>
+        <v>0.39527735000000003</v>
       </c>
       <c r="K58" s="4">
         <v>0.22367137723924296</v>
@@ -3037,7 +3037,7 @@
         <v>0.20058474364402323</v>
       </c>
       <c r="J59" s="6">
-        <v>0.39696767536640071</v>
+        <v>0.41781140999999999</v>
       </c>
       <c r="K59" s="4">
         <v>0.28086045668657861</v>
@@ -3081,7 +3081,7 @@
         <v>0.20370074668340621</v>
       </c>
       <c r="J60" s="6">
-        <v>0.36232391464428887</v>
+        <v>0.42713435999999999</v>
       </c>
       <c r="K60" s="4">
         <v>0.21375840664503271</v>
@@ -3125,7 +3125,7 @@
         <v>0.195182867279387</v>
       </c>
       <c r="J61" s="6">
-        <v>0.37156153885474419</v>
+        <v>0.38349720999999998</v>
       </c>
       <c r="K61" s="4">
         <v>0.19833758382130018</v>
@@ -3169,7 +3169,7 @@
         <v>0.20458023723844132</v>
       </c>
       <c r="J62" s="6">
-        <v>0.38647109315565714</v>
+        <v>0.38134031000000002</v>
       </c>
       <c r="K62" s="4">
         <v>0.19918644281214162</v>
@@ -3213,7 +3213,7 @@
         <v>0.19485818974543373</v>
       </c>
       <c r="J63" s="6">
-        <v>0.42493035090307413</v>
+        <v>0.40866543</v>
       </c>
       <c r="K63" s="4">
         <v>0.20685415549258976</v>
@@ -3257,7 +3257,7 @@
         <v>0.20285812115331051</v>
       </c>
       <c r="J64" s="6">
-        <v>0.44828876691237241</v>
+        <v>0.41288902</v>
       </c>
       <c r="K64" s="4">
         <v>0.19450218345839992</v>
@@ -3301,7 +3301,7 @@
         <v>0.20398363278667667</v>
       </c>
       <c r="J65" s="6">
-        <v>0.39467053502467886</v>
+        <v>0.40776774999999998</v>
       </c>
       <c r="K65" s="4">
         <v>5.6930252379334079E-2</v>
@@ -3345,7 +3345,7 @@
         <v>0.19642247721039316</v>
       </c>
       <c r="J66" s="6">
-        <v>0.39823121814992718</v>
+        <v>0.41932477000000001</v>
       </c>
       <c r="K66" s="4">
         <v>0.22504481019947223</v>
@@ -3389,7 +3389,7 @@
         <v>0.19878397439656004</v>
       </c>
       <c r="J67" s="6">
-        <v>0.3948925822398342</v>
+        <v>0.37267578000000001</v>
       </c>
       <c r="K67" s="4">
         <v>0.22847872181009374</v>
@@ -3433,7 +3433,7 @@
         <v>0.2108199014795033</v>
       </c>
       <c r="J68" s="6">
-        <v>0.38076093825869195</v>
+        <v>0.37519939000000002</v>
       </c>
       <c r="K68" s="4">
         <v>0.17428582235032639</v>
@@ -3477,7 +3477,7 @@
         <v>0.20745064074410091</v>
       </c>
       <c r="J69" s="6">
-        <v>0.3957063122950869</v>
+        <v>0.40140310000000001</v>
       </c>
       <c r="K69" s="4">
         <v>0.24414075462545118</v>
@@ -3521,7 +3521,7 @@
         <v>0.1952325863804083</v>
       </c>
       <c r="J70" s="6">
-        <v>0.44012150993543575</v>
+        <v>0.42975858</v>
       </c>
       <c r="K70" s="4">
         <v>0.16022860138621764</v>
@@ -3565,7 +3565,7 @@
         <v>0.18887651482704379</v>
       </c>
       <c r="J71" s="6">
-        <v>0.37343576554103175</v>
+        <v>0.36766106999999998</v>
       </c>
       <c r="K71" s="4">
         <v>0.17768686583576859</v>
@@ -3609,7 +3609,7 @@
         <v>0.19843739432864407</v>
       </c>
       <c r="J72" s="6">
-        <v>0.39776624821173662</v>
+        <v>0.38103273999999998</v>
       </c>
       <c r="K72" s="4">
         <v>0.24017257189545685</v>
@@ -3653,7 +3653,7 @@
         <v>0.19923394392473648</v>
       </c>
       <c r="J73" s="6">
-        <v>0.42074604301968616</v>
+        <v>0.40904712999999998</v>
       </c>
       <c r="K73" s="4">
         <v>0.11825453059586259</v>
@@ -3697,7 +3697,7 @@
         <v>0.1876314985263563</v>
       </c>
       <c r="J74" s="6">
-        <v>0.39467027637105379</v>
+        <v>0.40602439000000001</v>
       </c>
       <c r="K74" s="4">
         <v>0.26585112656376397</v>
@@ -3741,7 +3741,7 @@
         <v>0.19662815281975218</v>
       </c>
       <c r="J75" s="6">
-        <v>0.41696000745112377</v>
+        <v>0.39925479000000003</v>
       </c>
       <c r="K75" s="4">
         <v>0.1870808336221394</v>
@@ -3785,7 +3785,7 @@
         <v>0.19953166036919706</v>
       </c>
       <c r="J76" s="6">
-        <v>0.43352724827532113</v>
+        <v>0.43446654000000001</v>
       </c>
       <c r="K76" s="4">
         <v>0.17387676983005695</v>
@@ -3829,7 +3829,7 @@
         <v>0.18434332410790158</v>
       </c>
       <c r="J77" s="6">
-        <v>0.42186809136538816</v>
+        <v>0.38618373</v>
       </c>
       <c r="K77" s="4">
         <v>0.19143006988815103</v>
@@ -3873,7 +3873,7 @@
         <v>0.21028680877089223</v>
       </c>
       <c r="J78" s="6">
-        <v>0.37238974323338997</v>
+        <v>0.41454435000000001</v>
       </c>
       <c r="K78" s="4">
         <v>0.14601639494737167</v>
@@ -3917,7 +3917,7 @@
         <v>0.19368504744228512</v>
       </c>
       <c r="J79" s="6">
-        <v>0.39518556969017399</v>
+        <v>0.41062430999999999</v>
       </c>
       <c r="K79" s="4">
         <v>0.19963687958211376</v>
@@ -3961,7 +3961,7 @@
         <v>0.19979012190951995</v>
       </c>
       <c r="J80" s="6">
-        <v>0.41482314640187568</v>
+        <v>0.40530411</v>
       </c>
       <c r="K80" s="4">
         <v>0.19567090326687112</v>
@@ -4005,7 +4005,7 @@
         <v>0.19673306247729494</v>
       </c>
       <c r="J81" s="6">
-        <v>0.40440857488549903</v>
+        <v>0.42358910999999999</v>
       </c>
       <c r="K81" s="4">
         <v>0.22417493120794832</v>
@@ -4049,7 +4049,7 @@
         <v>0.18711820191222864</v>
       </c>
       <c r="J82" s="6">
-        <v>0.37175949690681087</v>
+        <v>0.42565935999999999</v>
       </c>
       <c r="K82" s="4">
         <v>0.21416383158423752</v>
@@ -4093,7 +4093,7 @@
         <v>0.17738438547510524</v>
       </c>
       <c r="J83" s="6">
-        <v>0.3979439234670728</v>
+        <v>0.36763529</v>
       </c>
       <c r="K83" s="4">
         <v>0.2020186015690742</v>
@@ -4137,7 +4137,7 @@
         <v>0.20625633895289855</v>
       </c>
       <c r="J84" s="6">
-        <v>0.38765815549607652</v>
+        <v>0.40242938</v>
       </c>
       <c r="K84" s="4">
         <v>0.20923856908255833</v>
@@ -4181,7 +4181,7 @@
         <v>0.18729507811175058</v>
       </c>
       <c r="J85" s="6">
-        <v>0.38871289559668026</v>
+        <v>0.38819095999999997</v>
       </c>
       <c r="K85" s="4">
         <v>0.29772443210945282</v>
@@ -4225,7 +4225,7 @@
         <v>0.20465036081317495</v>
       </c>
       <c r="J86" s="6">
-        <v>0.39163476275267334</v>
+        <v>0.42508016999999998</v>
       </c>
       <c r="K86" s="4">
         <v>0.21667921308464203</v>
@@ -4269,7 +4269,7 @@
         <v>0.20273148097359092</v>
       </c>
       <c r="J87" s="6">
-        <v>0.4209272502255279</v>
+        <v>0.41912972999999998</v>
       </c>
       <c r="K87" s="4">
         <v>0.20261061038637923</v>
@@ -4313,7 +4313,7 @@
         <v>0.19630511480154184</v>
       </c>
       <c r="J88" s="6">
-        <v>0.42537263735180342</v>
+        <v>0.45532863000000001</v>
       </c>
       <c r="K88" s="4">
         <v>0.23448627172687</v>
@@ -4357,7 +4357,7 @@
         <v>0.20595507784687089</v>
       </c>
       <c r="J89" s="6">
-        <v>0.45720499435793605</v>
+        <v>0.36818537000000001</v>
       </c>
       <c r="K89" s="4">
         <v>0.15166298794171071</v>
@@ -4401,7 +4401,7 @@
         <v>0.19602886044043435</v>
       </c>
       <c r="J90" s="6">
-        <v>0.37919546107807139</v>
+        <v>0.40851019</v>
       </c>
       <c r="K90" s="4">
         <v>0.16867531360435561</v>
@@ -4445,7 +4445,7 @@
         <v>0.19722348738035311</v>
       </c>
       <c r="J91" s="6">
-        <v>0.39553600352247731</v>
+        <v>0.42283310000000002</v>
       </c>
       <c r="K91" s="4">
         <v>0.20218942793052555</v>
@@ -4489,7 +4489,7 @@
         <v>0.21259830406081234</v>
       </c>
       <c r="J92" s="6">
-        <v>0.41163482620378683</v>
+        <v>0.40039288000000001</v>
       </c>
       <c r="K92" s="4">
         <v>0.22042592621844312</v>
@@ -4533,7 +4533,7 @@
         <v>0.1887535066177313</v>
       </c>
       <c r="J93" s="6">
-        <v>0.41956847652458767</v>
+        <v>0.36724285000000001</v>
       </c>
       <c r="K93" s="4">
         <v>0.18202653603786534</v>
@@ -4577,7 +4577,7 @@
         <v>0.18956042804859441</v>
       </c>
       <c r="J94" s="6">
-        <v>0.40073762709989802</v>
+        <v>0.40675721999999997</v>
       </c>
       <c r="K94" s="4">
         <v>0.26881605042674411</v>
@@ -4621,7 +4621,7 @@
         <v>0.2024583229903788</v>
       </c>
       <c r="J95" s="6">
-        <v>0.41276906214986686</v>
+        <v>0.40638680999999999</v>
       </c>
       <c r="K95" s="4">
         <v>0.249221091436852</v>
@@ -4665,7 +4665,7 @@
         <v>0.18387848510044441</v>
       </c>
       <c r="J96" s="6">
-        <v>0.40738840986039643</v>
+        <v>0.37461201</v>
       </c>
       <c r="K96" s="4">
         <v>0.21297849690729906</v>
@@ -4709,7 +4709,7 @@
         <v>0.1850514573382982</v>
       </c>
       <c r="J97" s="6">
-        <v>0.46104009907736831</v>
+        <v>0.40386727</v>
       </c>
       <c r="K97" s="4">
         <v>0.27428382427665687</v>
@@ -4753,7 +4753,7 @@
         <v>0.20849512885783267</v>
       </c>
       <c r="J98" s="6">
-        <v>0.37611413731271692</v>
+        <v>0.39699491999999997</v>
       </c>
       <c r="K98" s="4">
         <v>0.1633994048502794</v>
@@ -4797,7 +4797,7 @@
         <v>0.18895712976137638</v>
       </c>
       <c r="J99" s="6">
-        <v>0.42487556321922293</v>
+        <v>0.40233956999999998</v>
       </c>
       <c r="K99" s="4">
         <v>0.20210351129755802</v>
@@ -4841,7 +4841,7 @@
         <v>0.19132263904324187</v>
       </c>
       <c r="J100" s="6">
-        <v>0.39255655971280673</v>
+        <v>0.38849261000000002</v>
       </c>
       <c r="K100" s="4">
         <v>0.16942578397463987</v>
@@ -4885,7 +4885,7 @@
         <v>0.20120180006518695</v>
       </c>
       <c r="J101" s="6">
-        <v>0.3846588042580168</v>
+        <v>0.41115434000000001</v>
       </c>
       <c r="K101" s="4">
         <v>0.15551411157070491</v>
@@ -4929,7 +4929,7 @@
         <v>0.18617771205321795</v>
       </c>
       <c r="J102" s="6">
-        <v>0.41444339803554314</v>
+        <v>0.40014240000000001</v>
       </c>
       <c r="K102" s="4">
         <v>0.21938666484986535</v>
@@ -4973,7 +4973,7 @@
         <v>0.18718102861248506</v>
       </c>
       <c r="J103" s="6">
-        <v>0.39409811926273902</v>
+        <v>0.39217547000000003</v>
       </c>
       <c r="K103" s="4">
         <v>0.25574019252970026</v>
@@ -5017,7 +5017,7 @@
         <v>0.19038662238801204</v>
       </c>
       <c r="J104" s="6">
-        <v>0.38903214365176753</v>
+        <v>0.45529546999999998</v>
       </c>
       <c r="K104" s="4">
         <v>0.20367036012652895</v>
@@ -5061,7 +5061,7 @@
         <v>0.19597490584451929</v>
       </c>
       <c r="J105" s="6">
-        <v>0.40173025837103477</v>
+        <v>0.38964149999999997</v>
       </c>
       <c r="K105" s="4">
         <v>0.23698925577524024</v>
@@ -5105,7 +5105,7 @@
         <v>0.20729025842925852</v>
       </c>
       <c r="J106" s="6">
-        <v>0.37547734238273628</v>
+        <v>0.43274383999999999</v>
       </c>
       <c r="K106" s="4">
         <v>0.21404464322939329</v>
@@ -5149,7 +5149,7 @@
         <v>0.2111068752292331</v>
       </c>
       <c r="J107" s="6">
-        <v>0.38370764664080081</v>
+        <v>0.41959737000000003</v>
       </c>
       <c r="K107" s="4">
         <v>0.24029701426792607</v>
@@ -5193,7 +5193,7 @@
         <v>0.20730598770501824</v>
       </c>
       <c r="J108" s="6">
-        <v>0.38900160524080912</v>
+        <v>0.42620975999999999</v>
       </c>
       <c r="K108" s="4">
         <v>0.1881049595100569</v>
@@ -5237,7 +5237,7 @@
         <v>0.19619127194928579</v>
       </c>
       <c r="J109" s="6">
-        <v>0.39973373862719763</v>
+        <v>0.41330854</v>
       </c>
       <c r="K109" s="4">
         <v>0.14362703735133092</v>
@@ -5281,7 +5281,7 @@
         <v>0.1939240550960295</v>
       </c>
       <c r="J110" s="6">
-        <v>0.44950693763368882</v>
+        <v>0.39085341000000001</v>
       </c>
       <c r="K110" s="4">
         <v>0.20343775809819292</v>
@@ -5325,7 +5325,7 @@
         <v>0.19498972936071959</v>
       </c>
       <c r="J111" s="6">
-        <v>0.44281658750897995</v>
+        <v>0.41311055000000002</v>
       </c>
       <c r="K111" s="4">
         <v>0.2853109302090534</v>
@@ -5369,7 +5369,7 @@
         <v>0.2020293934766437</v>
       </c>
       <c r="J112" s="6">
-        <v>0.38619916559639172</v>
+        <v>0.41578904999999999</v>
       </c>
       <c r="K112" s="4">
         <v>0.19476682438455029</v>
@@ -5413,7 +5413,7 @@
         <v>0.21267922714601023</v>
       </c>
       <c r="J113" s="6">
-        <v>0.37509122123574024</v>
+        <v>0.37598256000000002</v>
       </c>
       <c r="K113" s="4">
         <v>0.18565389947128533</v>
@@ -5457,7 +5457,7 @@
         <v>0.19392183463889723</v>
       </c>
       <c r="J114" s="6">
-        <v>0.42847875482165226</v>
+        <v>0.39067679</v>
       </c>
       <c r="K114" s="4">
         <v>0.19770888769243228</v>
@@ -5501,7 +5501,7 @@
         <v>0.21496540658451635</v>
       </c>
       <c r="J115" s="6">
-        <v>0.40007719072074288</v>
+        <v>0.40879282</v>
       </c>
       <c r="K115" s="4">
         <v>0.2220158473862574</v>
@@ -5545,7 +5545,7 @@
         <v>0.19634098096075109</v>
       </c>
       <c r="J116" s="6">
-        <v>0.41760461737639115</v>
+        <v>0.39284604000000001</v>
       </c>
       <c r="K116" s="4">
         <v>0.20702300240042135</v>
@@ -5589,7 +5589,7 @@
         <v>0.20229766132201379</v>
       </c>
       <c r="J117" s="6">
-        <v>0.40733813341074493</v>
+        <v>0.38335729000000002</v>
       </c>
       <c r="K117" s="4">
         <v>0.18791461958545136</v>
@@ -5633,7 +5633,7 @@
         <v>0.18516518046476396</v>
       </c>
       <c r="J118" s="6">
-        <v>0.38882892502134281</v>
+        <v>0.39699187000000002</v>
       </c>
       <c r="K118" s="4">
         <v>0.20919122102175955</v>
@@ -5677,7 +5677,7 @@
         <v>0.18481620972306995</v>
       </c>
       <c r="J119" s="6">
-        <v>0.39318628449105736</v>
+        <v>0.40051978999999999</v>
       </c>
       <c r="K119" s="4">
         <v>0.22460644004757693</v>
@@ -5721,7 +5721,7 @@
         <v>0.19562361406380083</v>
       </c>
       <c r="J120" s="6">
-        <v>0.40921853554970472</v>
+        <v>0.44578769000000001</v>
       </c>
       <c r="K120" s="4">
         <v>0.15360143463595546</v>
@@ -5765,7 +5765,7 @@
         <v>0.1983607709707432</v>
       </c>
       <c r="J121" s="6">
-        <v>0.38804436219398475</v>
+        <v>0.37851358000000002</v>
       </c>
       <c r="K121" s="4">
         <v>0.18844254880465156</v>
@@ -5809,7 +5809,7 @@
         <v>0.20362149785881914</v>
       </c>
       <c r="J122" s="6">
-        <v>0.42575639491004452</v>
+        <v>0.41942404</v>
       </c>
       <c r="K122" s="4">
         <v>0.2608785616040592</v>
@@ -5853,7 +5853,7 @@
         <v>0.21178009005284373</v>
       </c>
       <c r="J123" s="6">
-        <v>0.39658060310320847</v>
+        <v>0.42000969999999999</v>
       </c>
       <c r="K123" s="4">
         <v>0.16963177653100564</v>
@@ -5897,7 +5897,7 @@
         <v>0.21880002132848195</v>
       </c>
       <c r="J124" s="6">
-        <v>0.3945627440017877</v>
+        <v>0.42124233</v>
       </c>
       <c r="K124" s="4">
         <v>0.23929901167112219</v>
@@ -5941,7 +5941,7 @@
         <v>0.17806009352938335</v>
       </c>
       <c r="J125" s="6">
-        <v>0.39211903349055921</v>
+        <v>0.38136916999999998</v>
       </c>
       <c r="K125" s="4">
         <v>0.16507343677608405</v>
@@ -5985,7 +5985,7 @@
         <v>0.20829023420117596</v>
       </c>
       <c r="J126" s="6">
-        <v>0.43784807823236827</v>
+        <v>0.36660559999999998</v>
       </c>
       <c r="K126" s="4">
         <v>0.2167274501757265</v>
@@ -6029,7 +6029,7 @@
         <v>0.1982856224256736</v>
       </c>
       <c r="J127" s="6">
-        <v>0.40467636004819091</v>
+        <v>0.37383981999999999</v>
       </c>
       <c r="K127" s="4">
         <v>0.20100771109090532</v>
@@ -6073,7 +6073,7 @@
         <v>0.22255137605646041</v>
       </c>
       <c r="J128" s="6">
-        <v>0.38652113458575932</v>
+        <v>0.41739978</v>
       </c>
       <c r="K128" s="4">
         <v>0.17649279422076231</v>
@@ -6117,7 +6117,7 @@
         <v>0.20491330939002739</v>
       </c>
       <c r="J129" s="6">
-        <v>0.35751958425202474</v>
+        <v>0.41604340000000001</v>
       </c>
       <c r="K129" s="4">
         <v>0.29843395467076944</v>
@@ -6161,7 +6161,7 @@
         <v>0.18565331128965576</v>
       </c>
       <c r="J130" s="6">
-        <v>0.42043299595144218</v>
+        <v>0.42323954000000003</v>
       </c>
       <c r="K130" s="4">
         <v>0.15751580311917118</v>
@@ -6205,7 +6205,7 @@
         <v>0.19989606240323135</v>
       </c>
       <c r="J131" s="6">
-        <v>0.39059807074774927</v>
+        <v>0.41050776999999999</v>
       </c>
       <c r="K131" s="4">
         <v>0.20496455686371576</v>
@@ -6249,7 +6249,7 @@
         <v>0.20194109499709292</v>
       </c>
       <c r="J132" s="6">
-        <v>0.41172044707346145</v>
+        <v>0.40731012999999999</v>
       </c>
       <c r="K132" s="4">
         <v>0.16860011226369342</v>
@@ -6293,7 +6293,7 @@
         <v>0.20053313130053704</v>
       </c>
       <c r="J133" s="6">
-        <v>0.411249519203714</v>
+        <v>0.42834243</v>
       </c>
       <c r="K133" s="4">
         <v>0.17738978707690942</v>
@@ -6337,7 +6337,7 @@
         <v>0.2085519360220135</v>
       </c>
       <c r="J134" s="6">
-        <v>0.39060803036829167</v>
+        <v>0.39385046000000001</v>
       </c>
       <c r="K134" s="4">
         <v>0.20279380795796403</v>
@@ -6381,7 +6381,7 @@
         <v>0.19711760858328345</v>
       </c>
       <c r="J135" s="6">
-        <v>0.37405271495622849</v>
+        <v>0.40419706</v>
       </c>
       <c r="K135" s="4">
         <v>0.23505021149873012</v>
@@ -6425,7 +6425,7 @@
         <v>0.19174159273772892</v>
       </c>
       <c r="J136" s="6">
-        <v>0.41878311983647826</v>
+        <v>0.35359391000000001</v>
       </c>
       <c r="K136" s="4">
         <v>0.24845452469801502</v>
@@ -6469,7 +6469,7 @@
         <v>0.17711774037591943</v>
       </c>
       <c r="J137" s="6">
-        <v>0.4066700697600924</v>
+        <v>0.38980123</v>
       </c>
       <c r="K137" s="4">
         <v>0.22648095902388105</v>
@@ -6513,7 +6513,7 @@
         <v>0.20517375486153958</v>
       </c>
       <c r="J138" s="6">
-        <v>0.39524201604158798</v>
+        <v>0.37153668000000001</v>
       </c>
       <c r="K138" s="4">
         <v>0.24590823106987847</v>
@@ -6557,7 +6557,7 @@
         <v>0.19371124766531186</v>
       </c>
       <c r="J139" s="6">
-        <v>0.43501406278765364</v>
+        <v>0.42690904000000002</v>
       </c>
       <c r="K139" s="4">
         <v>0.16313775679576584</v>
@@ -6601,7 +6601,7 @@
         <v>0.1977332598341644</v>
       </c>
       <c r="J140" s="6">
-        <v>0.40855255115545497</v>
+        <v>0.39375374000000002</v>
       </c>
       <c r="K140" s="4">
         <v>0.24726239843672074</v>
@@ -6645,7 +6645,7 @@
         <v>0.20151401497097121</v>
       </c>
       <c r="J141" s="6">
-        <v>0.37596249455306063</v>
+        <v>0.40760793000000001</v>
       </c>
       <c r="K141" s="4">
         <v>0.18015077671255947</v>
@@ -6689,7 +6689,7 @@
         <v>0.20058344473658621</v>
       </c>
       <c r="J142" s="6">
-        <v>0.37566330358109307</v>
+        <v>0.40953412</v>
       </c>
       <c r="K142" s="4">
         <v>0.24411447671273778</v>
@@ -6733,7 +6733,7 @@
         <v>0.2157980172328714</v>
       </c>
       <c r="J143" s="6">
-        <v>0.3763323214383697</v>
+        <v>0.39210884000000001</v>
       </c>
       <c r="K143" s="4">
         <v>0.23512156020082597</v>
@@ -6777,7 +6777,7 @@
         <v>0.20663397799329494</v>
       </c>
       <c r="J144" s="6">
-        <v>0.37369612050125228</v>
+        <v>0.39251647000000001</v>
       </c>
       <c r="K144" s="4">
         <v>0.25773093747911424</v>
@@ -6821,7 +6821,7 @@
         <v>0.20139960767782372</v>
       </c>
       <c r="J145" s="6">
-        <v>0.41049724345486233</v>
+        <v>0.39295911</v>
       </c>
       <c r="K145" s="4">
         <v>0.16597382257059351</v>
@@ -6865,7 +6865,7 @@
         <v>0.18474983201503953</v>
       </c>
       <c r="J146" s="6">
-        <v>0.42901013544834693</v>
+        <v>0.40406247000000001</v>
       </c>
       <c r="K146" s="4">
         <v>0.24166589087818635</v>
@@ -6909,7 +6909,7 @@
         <v>0.20838034132254477</v>
       </c>
       <c r="J147" s="6">
-        <v>0.40100308653501754</v>
+        <v>0.38774773000000001</v>
       </c>
       <c r="K147" s="4">
         <v>0.1642949337514277</v>
@@ -6953,7 +6953,7 @@
         <v>0.21304691142846982</v>
       </c>
       <c r="J148" s="6">
-        <v>0.38946472181867026</v>
+        <v>0.42108811000000002</v>
       </c>
       <c r="K148" s="4">
         <v>0.17173136326942023</v>
@@ -6997,7 +6997,7 @@
         <v>0.19552537998722203</v>
       </c>
       <c r="J149" s="6">
-        <v>0.40622778010655086</v>
+        <v>0.41021663000000003</v>
       </c>
       <c r="K149" s="4">
         <v>0.2067796194751306</v>
@@ -7041,7 +7041,7 @@
         <v>0.19034100353205025</v>
       </c>
       <c r="J150" s="6">
-        <v>0.38381867292134275</v>
+        <v>0.41903027999999998</v>
       </c>
       <c r="K150" s="4">
         <v>0.28362393634756439</v>
@@ -7085,7 +7085,7 @@
         <v>0.19669633991711286</v>
       </c>
       <c r="J151" s="6">
-        <v>0.38082030922785742</v>
+        <v>0.37403314999999998</v>
       </c>
       <c r="K151" s="4">
         <v>0.22049347921553239</v>
@@ -7129,7 +7129,7 @@
         <v>0.21616130092811908</v>
       </c>
       <c r="J152" s="6">
-        <v>0.38088330979446383</v>
+        <v>0.38269605000000001</v>
       </c>
       <c r="K152" s="4">
         <v>0.23209532406922867</v>
@@ -7173,7 +7173,7 @@
         <v>0.20112759539615704</v>
       </c>
       <c r="J153" s="6">
-        <v>0.42406373873273506</v>
+        <v>0.40621299</v>
       </c>
       <c r="K153" s="4">
         <v>0.24177140420192705</v>
@@ -7217,7 +7217,7 @@
         <v>0.18807273535758923</v>
       </c>
       <c r="J154" s="6">
-        <v>0.43647965909863712</v>
+        <v>0.40434514999999999</v>
       </c>
       <c r="K154" s="4">
         <v>0.17471269737325412</v>
@@ -7261,7 +7261,7 @@
         <v>0.20314118156945379</v>
       </c>
       <c r="J155" s="6">
-        <v>0.41650947366543628</v>
+        <v>0.37818164999999998</v>
       </c>
       <c r="K155" s="4">
         <v>0.1834516736752988</v>
@@ -7305,7 +7305,7 @@
         <v>0.19141354712471254</v>
       </c>
       <c r="J156" s="6">
-        <v>0.40722211106379308</v>
+        <v>0.42959391000000002</v>
       </c>
       <c r="K156" s="4">
         <v>0.22676818542230656</v>
@@ -7349,7 +7349,7 @@
         <v>0.20410356368741114</v>
       </c>
       <c r="J157" s="6">
-        <v>0.39181075504821439</v>
+        <v>0.39920636999999998</v>
       </c>
       <c r="K157" s="4">
         <v>0.19327852903337644</v>
@@ -7393,7 +7393,7 @@
         <v>0.21401992306108664</v>
       </c>
       <c r="J158" s="6">
-        <v>0.39421046784344577</v>
+        <v>0.38677401</v>
       </c>
       <c r="K158" s="4">
         <v>0.1570989870416967</v>
@@ -7437,7 +7437,7 @@
         <v>0.18267505832946235</v>
       </c>
       <c r="J159" s="6">
-        <v>0.41160476081776032</v>
+        <v>0.41035112000000001</v>
       </c>
       <c r="K159" s="4">
         <v>0.24122591235867313</v>
@@ -7481,7 +7481,7 @@
         <v>0.1890251803768698</v>
       </c>
       <c r="J160" s="6">
-        <v>0.37950798330274793</v>
+        <v>0.35867007000000001</v>
       </c>
       <c r="K160" s="4">
         <v>0.24440781505892623</v>
@@ -7525,7 +7525,7 @@
         <v>0.19944494151551184</v>
       </c>
       <c r="J161" s="6">
-        <v>0.42907765592599584</v>
+        <v>0.37984402</v>
       </c>
       <c r="K161" s="4">
         <v>0.20093813335694685</v>
@@ -7569,7 +7569,7 @@
         <v>0.19039704408334301</v>
       </c>
       <c r="J162" s="6">
-        <v>0.3916449829856461</v>
+        <v>0.37422941999999998</v>
       </c>
       <c r="K162" s="4">
         <v>0.14276075889636991</v>
@@ -7613,7 +7613,7 @@
         <v>0.18344308059128492</v>
       </c>
       <c r="J163" s="6">
-        <v>0.35788576550005097</v>
+        <v>0.42999469000000001</v>
       </c>
       <c r="K163" s="4">
         <v>0.21631821978891519</v>
@@ -7657,7 +7657,7 @@
         <v>0.20546838960656041</v>
       </c>
       <c r="J164" s="6">
-        <v>0.37185077173343217</v>
+        <v>0.42135223999999999</v>
       </c>
       <c r="K164" s="4">
         <v>0.19020856618506193</v>
@@ -7701,7 +7701,7 @@
         <v>0.20119826344329525</v>
       </c>
       <c r="J165" s="6">
-        <v>0.42185276559715423</v>
+        <v>0.41429764000000002</v>
       </c>
       <c r="K165" s="4">
         <v>0.21829135774143393</v>
@@ -7745,7 +7745,7 @@
         <v>0.20873706917942167</v>
       </c>
       <c r="J166" s="6">
-        <v>0.38787879700709549</v>
+        <v>0.41585253999999999</v>
       </c>
       <c r="K166" s="4">
         <v>0.246720826778589</v>
@@ -7789,7 +7789,7 @@
         <v>0.19283360232365532</v>
       </c>
       <c r="J167" s="6">
-        <v>0.37835660762724932</v>
+        <v>0.43717056999999998</v>
       </c>
       <c r="K167" s="4">
         <v>0.14221741779930844</v>
@@ -7833,7 +7833,7 @@
         <v>0.20147037130093939</v>
       </c>
       <c r="J168" s="6">
-        <v>0.39058070423410068</v>
+        <v>0.39896431999999998</v>
       </c>
       <c r="K168" s="4">
         <v>0.20648506709298031</v>
@@ -7877,7 +7877,7 @@
         <v>0.21773503682560849</v>
       </c>
       <c r="J169" s="6">
-        <v>0.375561337055836</v>
+        <v>0.38798038000000001</v>
       </c>
       <c r="K169" s="4">
         <v>0.19418447678149031</v>
@@ -7921,7 +7921,7 @@
         <v>0.21272453510123104</v>
       </c>
       <c r="J170" s="6">
-        <v>0.42645593175841928</v>
+        <v>0.37959811999999998</v>
       </c>
       <c r="K170" s="4">
         <v>0.20771353222374214</v>
@@ -7965,7 +7965,7 @@
         <v>0.20650693011582638</v>
       </c>
       <c r="J171" s="6">
-        <v>0.38319760721572343</v>
+        <v>0.36789101000000002</v>
       </c>
       <c r="K171" s="4">
         <v>0.21221694399049448</v>
@@ -8009,7 +8009,7 @@
         <v>0.1859866296479174</v>
       </c>
       <c r="J172" s="6">
-        <v>0.41248311821177264</v>
+        <v>0.41067917999999998</v>
       </c>
       <c r="K172" s="4">
         <v>0.16393909705361709</v>
@@ -8053,7 +8053,7 @@
         <v>0.21948316320211503</v>
       </c>
       <c r="J173" s="6">
-        <v>0.38949998254343299</v>
+        <v>0.41334580999999998</v>
       </c>
       <c r="K173" s="4">
         <v>0.29237765660938725</v>
@@ -8097,7 +8097,7 @@
         <v>0.20578329585327115</v>
       </c>
       <c r="J174" s="6">
-        <v>0.36237516816353321</v>
+        <v>0.40282151999999999</v>
       </c>
       <c r="K174" s="4">
         <v>0.2108762872167278</v>
@@ -8141,7 +8141,7 @@
         <v>0.19034524505527448</v>
       </c>
       <c r="J175" s="6">
-        <v>0.40427298920500293</v>
+        <v>0.38632259000000002</v>
       </c>
       <c r="K175" s="4">
         <v>0.26469363013455433</v>
@@ -8185,7 +8185,7 @@
         <v>0.20238620995107709</v>
       </c>
       <c r="J176" s="6">
-        <v>0.4225602283893522</v>
+        <v>0.36461703000000001</v>
       </c>
       <c r="K176" s="4">
         <v>0.25927944697486288</v>
@@ -8229,7 +8229,7 @@
         <v>0.18089704831681569</v>
       </c>
       <c r="J177" s="6">
-        <v>0.39846567356432261</v>
+        <v>0.39878954</v>
       </c>
       <c r="K177" s="4">
         <v>0.21624205780985969</v>
@@ -8273,7 +8273,7 @@
         <v>0.20572743709301455</v>
       </c>
       <c r="J178" s="6">
-        <v>0.39220574912944367</v>
+        <v>0.39622114000000003</v>
       </c>
       <c r="K178" s="4">
         <v>0.21486622333538238</v>
@@ -8317,7 +8317,7 @@
         <v>0.19599128255880496</v>
       </c>
       <c r="J179" s="6">
-        <v>0.41494181492164556</v>
+        <v>0.36142289999999999</v>
       </c>
       <c r="K179" s="4">
         <v>0.19801387822305294</v>
@@ -8361,7 +8361,7 @@
         <v>0.2175313877461971</v>
       </c>
       <c r="J180" s="6">
-        <v>0.41006292949388434</v>
+        <v>0.37574034000000001</v>
       </c>
       <c r="K180" s="4">
         <v>0.20962713717658638</v>
@@ -8405,7 +8405,7 @@
         <v>0.20221012983116229</v>
       </c>
       <c r="J181" s="6">
-        <v>0.41893527096039779</v>
+        <v>0.38282328999999998</v>
       </c>
       <c r="K181" s="4">
         <v>0.1848613458011607</v>
@@ -8449,7 +8449,7 @@
         <v>0.19246924738153121</v>
       </c>
       <c r="J182" s="6">
-        <v>0.38675318470432485</v>
+        <v>0.35879966000000002</v>
       </c>
       <c r="K182" s="4">
         <v>0.21081329748115438</v>
@@ -8493,7 +8493,7 @@
         <v>0.17869537396911794</v>
       </c>
       <c r="J183" s="6">
-        <v>0.39274857827180337</v>
+        <v>0.39491483999999999</v>
       </c>
       <c r="K183" s="4">
         <v>0.25410079051035223</v>
@@ -8537,7 +8537,7 @@
         <v>0.19059317434926151</v>
       </c>
       <c r="J184" s="6">
-        <v>0.39989604464047018</v>
+        <v>0.40226498999999999</v>
       </c>
       <c r="K184" s="4">
         <v>0.14947667118434765</v>
@@ -8581,7 +8581,7 @@
         <v>0.17330192398672872</v>
       </c>
       <c r="J185" s="6">
-        <v>0.40647948167712222</v>
+        <v>0.39424029999999999</v>
       </c>
       <c r="K185" s="4">
         <v>0.20118250177896002</v>
@@ -8625,7 +8625,7 @@
         <v>0.18682742903138316</v>
       </c>
       <c r="J186" s="6">
-        <v>0.36662919626878843</v>
+        <v>0.39057972000000002</v>
       </c>
       <c r="K186" s="4">
         <v>0.18729712029670886</v>
@@ -8669,7 +8669,7 @@
         <v>0.20000115201792934</v>
       </c>
       <c r="J187" s="6">
-        <v>0.4047240756707276</v>
+        <v>0.37500704000000001</v>
       </c>
       <c r="K187" s="4">
         <v>0.20854211389865773</v>
@@ -8713,7 +8713,7 @@
         <v>0.21576682799126851</v>
       </c>
       <c r="J188" s="6">
-        <v>0.3518057402241716</v>
+        <v>0.37740019000000002</v>
       </c>
       <c r="K188" s="4">
         <v>0.21729311674402996</v>
@@ -8757,7 +8757,7 @@
         <v>0.19536291770656813</v>
       </c>
       <c r="J189" s="6">
-        <v>0.4345556553851907</v>
+        <v>0.38159546</v>
       </c>
       <c r="K189" s="4">
         <v>0.24826450207532588</v>
@@ -8801,7 +8801,7 @@
         <v>0.20112661315463443</v>
       </c>
       <c r="J190" s="6">
-        <v>0.38793965989811363</v>
+        <v>0.41069299999999997</v>
       </c>
       <c r="K190" s="4">
         <v>0.21072698989311556</v>
@@ -8845,7 +8845,7 @@
         <v>0.18639718185990767</v>
       </c>
       <c r="J191" s="6">
-        <v>0.40703779001875379</v>
+        <v>0.40422563</v>
       </c>
       <c r="K191" s="4">
         <v>0.20067183678943448</v>
@@ -8889,7 +8889,7 @@
         <v>0.20367506026377932</v>
       </c>
       <c r="J192" s="6">
-        <v>0.41570893871816006</v>
+        <v>0.37991049999999998</v>
       </c>
       <c r="K192" s="4">
         <v>0.21334631414057004</v>
@@ -8933,7 +8933,7 @@
         <v>0.20436259959900177</v>
       </c>
       <c r="J193" s="6">
-        <v>0.38706653738410479</v>
+        <v>0.41361060999999999</v>
       </c>
       <c r="K193" s="4">
         <v>0.24287391190809773</v>
@@ -8977,7 +8977,7 @@
         <v>0.22026094216787045</v>
       </c>
       <c r="J194" s="6">
-        <v>0.40949590750067227</v>
+        <v>0.38356636</v>
       </c>
       <c r="K194" s="4">
         <v>0.15188758874986344</v>
@@ -9021,7 +9021,7 @@
         <v>0.20249451362819607</v>
       </c>
       <c r="J195" s="6">
-        <v>0.37561720251356828</v>
+        <v>0.41390444999999998</v>
       </c>
       <c r="K195" s="4">
         <v>0.17333222601716664</v>
@@ -9065,7 +9065,7 @@
         <v>0.20029106678765596</v>
       </c>
       <c r="J196" s="6">
-        <v>0.39644809440584056</v>
+        <v>0.39400747000000003</v>
       </c>
       <c r="K196" s="4">
         <v>0.26758253192299541</v>
@@ -9109,7 +9109,7 @@
         <v>0.18849807138918356</v>
       </c>
       <c r="J197" s="6">
-        <v>0.41599208194218568</v>
+        <v>0.35519336000000001</v>
       </c>
       <c r="K197" s="4">
         <v>0.22890656301055598</v>
@@ -9153,7 +9153,7 @@
         <v>0.22424909610667598</v>
       </c>
       <c r="J198" s="6">
-        <v>0.41502336768390324</v>
+        <v>0.37049989</v>
       </c>
       <c r="K198" s="4">
         <v>0.23250479303189642</v>

</xml_diff>